<commit_message>
Migrated all content from local project folder
</commit_message>
<xml_diff>
--- a/Workspace/Draft/registre de faits.xlsx
+++ b/Workspace/Draft/registre de faits.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ECA817-4941-43B3-9387-D795A8573F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AFCB7A-4628-42C9-831E-AF6071F8917E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Sources" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Qui</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Le Raptor; michel</t>
-  </si>
-  <si>
-    <t>1 - Sources'!A10</t>
   </si>
 </sst>
 </file>
@@ -813,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,9 +852,7 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -936,9 +931,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" location="'1 - Sources'!A10" display="'1 - Sources'!A10" xr:uid="{B80E1E48-3D2D-466C-9F6C-61BCED68E4CE}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -949,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A7DD54-4937-46AF-91E1-991D61AD55EA}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>